<commit_message>
Completed analysis of Alt1
</commit_message>
<xml_diff>
--- a/Excel_Challenge_591 - Sum of Numbers following Hashes.xlsx
+++ b/Excel_Challenge_591 - Sum of Numbers following Hashes.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2466DB98-C036-4A9D-954F-23C3E45911B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30343F8-042C-4383-B96C-DE8D1DC85659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="Alt1" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_r">'Alt1'!$H$5</definedName>
+    <definedName name="_s">'Alt1'!$H$6</definedName>
+    <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
+  </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
   <si>
     <t>Data</t>
   </si>
@@ -49,12 +77,18 @@
   <si>
     <t>https://www.linkedin.com/in/excelbi/recent-activity/all/</t>
   </si>
+  <si>
+    <t>_r</t>
+  </si>
+  <si>
+    <t>_s</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,8 +104,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -90,6 +139,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -100,8 +155,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -109,8 +166,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Intro_Hd" xfId="2" xr:uid="{5C525A15-4D72-4C06-9E87-37915275BA3F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{0E192D20-BF9A-4F7F-88C5-0BBAC9D0D381}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -290,6 +349,77 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>55880</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>424180</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CF65573-0B0D-4D1A-9852-957D87625990}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2311400" y="53340"/>
+          <a:ext cx="2197100" cy="541020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1200" b="1" kern="1200"/>
+            <a:t>Fill in the # by sum of numbers following the #.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -556,11 +686,38 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="967" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{7723F811-0518-4CF8-BF5A-1F1365669519}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -736,4 +893,511 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CECBB9-3929-416D-8B3A-499B5792C4D3}">
+  <dimension ref="A1:K24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>33</v>
+      </c>
+      <c r="B3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>112</v>
+      </c>
+      <c r="E5" cm="1">
+        <f t="array" ref="E5:E23">_xlfn.LET(
+    _xlpm.c, A2:A20,
+    _xlpm.r, ROWS(_xlpm.c),
+    _xlpm.s, _xlfn.SEQUENCE(_xlpm.r, , _xlpm.r, -1),
+    IF(
+        _xlpm.c = "#",
+        INDEX(_xlfn.SCAN(0, INDEX(_xlpm.c, _xlpm.s), _xlfn.LAMBDA(_xlpm.a,_xlpm.x, IF(_xlpm.x = "#", , _xlpm.a + _xlpm.x))), _xlpm.s - 1),
+        _xlpm.c
+    )
+)</f>
+        <v>73</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5">
+        <f>ROWS(A2:A20)</f>
+        <v>19</v>
+      </c>
+      <c r="K5" cm="1">
+        <f t="array" ref="K5:K23" xml:space="preserve">
+_xlfn.LET(_xlpm.c, A2:A20,
+    _xlpm.r, ROWS(_xlpm.c),
+    _xlpm.s, _xlfn.SEQUENCE(_xlpm.r,,_xlpm.r,-1),
+    IF(
+        _xlpm.c = "#",
+        INDEX(_xlfn.SCAN(0, INDEX(_xlpm.c,_xlfn.ANCHORARRAY( _s)), _xlfn.LAMBDA(_xlpm.a,_xlpm.x, IF(_xlpm.x = "#", , _xlpm.a + _xlpm.x))), _xlpm.s - 1),
+        _xlpm.c
+    ))</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>54</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" cm="1">
+        <f t="array" ref="H6:H24">_xlfn.SEQUENCE(_r,,_r,-1)</f>
+        <v>19</v>
+      </c>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6:I24">INDEX(A2:A20,_xlfn.ANCHORARRAY(_s))</f>
+        <v>27</v>
+      </c>
+      <c r="J6" cm="1">
+        <f t="array" ref="J6:J24">_xlfn.SCAN(0,_xlfn.ANCHORARRAY( I6), _xlfn.LAMBDA(_xlpm.a,_xlpm.x, IF(_xlpm.x = "#", , _xlpm.a + _xlpm.x)))</f>
+        <v>27</v>
+      </c>
+      <c r="K6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>22</v>
+      </c>
+      <c r="E7">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>57</v>
+      </c>
+      <c r="J7">
+        <v>84</v>
+      </c>
+      <c r="K7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>36</v>
+      </c>
+      <c r="B8">
+        <v>36</v>
+      </c>
+      <c r="E8">
+        <v>112</v>
+      </c>
+      <c r="H8">
+        <v>17</v>
+      </c>
+      <c r="I8">
+        <v>54</v>
+      </c>
+      <c r="J8">
+        <v>138</v>
+      </c>
+      <c r="K8">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>216</v>
+      </c>
+      <c r="E9">
+        <v>54</v>
+      </c>
+      <c r="H9">
+        <v>16</v>
+      </c>
+      <c r="I9" t="str">
+        <v>#</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
+      <c r="I10">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>53</v>
+      </c>
+      <c r="K10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>54</v>
+      </c>
+      <c r="B11">
+        <v>54</v>
+      </c>
+      <c r="E11">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <v>14</v>
+      </c>
+      <c r="I11" t="str">
+        <v>#</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>64</v>
+      </c>
+      <c r="E12">
+        <v>216</v>
+      </c>
+      <c r="H12">
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <v>54</v>
+      </c>
+      <c r="J12">
+        <v>54</v>
+      </c>
+      <c r="K12">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <v>34</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>12</v>
+      </c>
+      <c r="I13">
+        <v>34</v>
+      </c>
+      <c r="J13">
+        <v>88</v>
+      </c>
+      <c r="K13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>54</v>
+      </c>
+      <c r="B14">
+        <v>54</v>
+      </c>
+      <c r="E14">
+        <v>54</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+      <c r="I14">
+        <v>64</v>
+      </c>
+      <c r="J14">
+        <v>152</v>
+      </c>
+      <c r="K14">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>53</v>
+      </c>
+      <c r="E15">
+        <v>64</v>
+      </c>
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <v>54</v>
+      </c>
+      <c r="J15">
+        <v>206</v>
+      </c>
+      <c r="K15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <v>34</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="I16">
+        <v>10</v>
+      </c>
+      <c r="J16">
+        <v>216</v>
+      </c>
+      <c r="K16">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>138</v>
+      </c>
+      <c r="E17">
+        <v>54</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17" t="str">
+        <v>#</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>54</v>
+      </c>
+      <c r="B18">
+        <v>54</v>
+      </c>
+      <c r="E18">
+        <v>53</v>
+      </c>
+      <c r="H18">
+        <v>7</v>
+      </c>
+      <c r="I18">
+        <v>36</v>
+      </c>
+      <c r="J18">
+        <v>36</v>
+      </c>
+      <c r="K18">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>53</v>
+      </c>
+      <c r="H19">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>22</v>
+      </c>
+      <c r="J19">
+        <v>58</v>
+      </c>
+      <c r="K19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>27</v>
+      </c>
+      <c r="E20">
+        <v>138</v>
+      </c>
+      <c r="H20">
+        <v>5</v>
+      </c>
+      <c r="I20">
+        <v>54</v>
+      </c>
+      <c r="J20">
+        <v>112</v>
+      </c>
+      <c r="K20">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>54</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21" t="str">
+        <v>#</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>57</v>
+      </c>
+      <c r="H22">
+        <v>3</v>
+      </c>
+      <c r="I22">
+        <v>40</v>
+      </c>
+      <c r="J22">
+        <v>40</v>
+      </c>
+      <c r="K22">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="E23">
+        <v>27</v>
+      </c>
+      <c r="H23">
+        <v>2</v>
+      </c>
+      <c r="I23">
+        <v>33</v>
+      </c>
+      <c r="J23">
+        <v>73</v>
+      </c>
+      <c r="K23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24" t="str">
+        <v>#</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Decided to do a detailed breakdown
</commit_message>
<xml_diff>
--- a/Excel_Challenge_591 - Sum of Numbers following Hashes.xlsx
+++ b/Excel_Challenge_591 - Sum of Numbers following Hashes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30343F8-042C-4383-B96C-DE8D1DC85659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B3EE52-383C-446D-9AF2-510D9ABB7E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -897,10 +897,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CECBB9-3929-416D-8B3A-499B5792C4D3}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,7 +908,7 @@
     <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -919,7 +919,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -927,7 +927,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>33</v>
       </c>
@@ -935,7 +935,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>40</v>
       </c>
@@ -943,7 +943,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -970,8 +970,38 @@
         <f>ROWS(A2:A20)</f>
         <v>19</v>
       </c>
-      <c r="K5" cm="1">
-        <f t="array" ref="K5:K23" xml:space="preserve">
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>54</v>
+      </c>
+      <c r="B6">
+        <v>54</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" cm="1">
+        <f t="array" ref="H6:H24">_xlfn.SEQUENCE(_r,,_r,-1)</f>
+        <v>19</v>
+      </c>
+      <c r="I6" cm="1">
+        <f t="array" ref="I6:I24">INDEX(A2:A20,_xlfn.ANCHORARRAY(_s))</f>
+        <v>27</v>
+      </c>
+      <c r="J6" cm="1">
+        <f t="array" ref="J6:J24">_xlfn.SCAN(0,_xlfn.ANCHORARRAY( I6), _xlfn.LAMBDA(_xlpm.a,_xlpm.x, IF(_xlpm.x = "#", , _xlpm.a + _xlpm.x)))</f>
+        <v>27</v>
+      </c>
+      <c r="K6" cm="1">
+        <f t="array" ref="K6:K24">IF(A2:A20="#",INDEX(_xlfn.ANCHORARRAY(J6),_xlfn.ANCHORARRAY(_s)-1),A2:A20)</f>
+        <v>73</v>
+      </c>
+      <c r="N6" cm="1">
+        <f t="array" ref="N6:N24" xml:space="preserve">
 _xlfn.LET(_xlpm.c, A2:A20,
     _xlpm.r, ROWS(_xlpm.c),
     _xlpm.s, _xlfn.SEQUENCE(_xlpm.r,,_xlpm.r,-1),
@@ -983,36 +1013,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>54</v>
-      </c>
-      <c r="B6">
-        <v>54</v>
-      </c>
-      <c r="E6">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" cm="1">
-        <f t="array" ref="H6:H24">_xlfn.SEQUENCE(_r,,_r,-1)</f>
-        <v>19</v>
-      </c>
-      <c r="I6" cm="1">
-        <f t="array" ref="I6:I24">INDEX(A2:A20,_xlfn.ANCHORARRAY(_s))</f>
-        <v>27</v>
-      </c>
-      <c r="J6" cm="1">
-        <f t="array" ref="J6:J24">_xlfn.SCAN(0,_xlfn.ANCHORARRAY( I6), _xlfn.LAMBDA(_xlpm.a,_xlpm.x, IF(_xlpm.x = "#", , _xlpm.a + _xlpm.x)))</f>
-        <v>27</v>
-      </c>
-      <c r="K6">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>22</v>
       </c>
@@ -1032,10 +1033,13 @@
         <v>84</v>
       </c>
       <c r="K7">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="N7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>36</v>
       </c>
@@ -1055,10 +1059,13 @@
         <v>138</v>
       </c>
       <c r="K8">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="N8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1078,10 +1085,13 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+      <c r="N9">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1101,10 +1111,13 @@
         <v>53</v>
       </c>
       <c r="K10">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="N10">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>54</v>
       </c>
@@ -1124,10 +1137,13 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="N11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>64</v>
       </c>
@@ -1147,10 +1163,13 @@
         <v>54</v>
       </c>
       <c r="K12">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="N12">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>34</v>
       </c>
@@ -1170,10 +1189,13 @@
         <v>88</v>
       </c>
       <c r="K13">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+      <c r="N13">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>54</v>
       </c>
@@ -1193,10 +1215,13 @@
         <v>152</v>
       </c>
       <c r="K14">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1216,10 +1241,13 @@
         <v>206</v>
       </c>
       <c r="K15">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="N15">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>53</v>
       </c>
@@ -1239,10 +1267,13 @@
         <v>216</v>
       </c>
       <c r="K16">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="N16">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1262,10 +1293,13 @@
         <v>0</v>
       </c>
       <c r="K17">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="N17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>54</v>
       </c>
@@ -1285,10 +1319,13 @@
         <v>36</v>
       </c>
       <c r="K18">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="N18">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>57</v>
       </c>
@@ -1310,8 +1347,11 @@
       <c r="K19">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="N19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>27</v>
       </c>
@@ -1331,10 +1371,13 @@
         <v>112</v>
       </c>
       <c r="K20">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+      <c r="N20">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E21">
         <v>54</v>
       </c>
@@ -1348,10 +1391,13 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="N21">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E22">
         <v>57</v>
       </c>
@@ -1365,10 +1411,13 @@
         <v>40</v>
       </c>
       <c r="K22">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="N22">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E23">
         <v>27</v>
       </c>
@@ -1382,10 +1431,13 @@
         <v>73</v>
       </c>
       <c r="K23">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+      <c r="N23">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>1</v>
       </c>
@@ -1394,6 +1446,12 @@
       </c>
       <c r="J24">
         <v>0</v>
+      </c>
+      <c r="K24">
+        <v>27</v>
+      </c>
+      <c r="N24">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>